<commit_message>
Pushing our actual responsiblilties chart.
</commit_message>
<xml_diff>
--- a/documentation/Enrollment Group 3 Class Schedule.xlsx
+++ b/documentation/Enrollment Group 3 Class Schedule.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>Task ID</t>
   </si>
@@ -49,7 +49,7 @@
     <t>Nathan, Stephen</t>
   </si>
   <si>
-    <t>In process</t>
+    <t>Completed</t>
   </si>
   <si>
     <t>N/A</t>
@@ -64,7 +64,7 @@
     <t>Develop functionality to manage class information such as course name, number, professor, and schedule.</t>
   </si>
   <si>
-    <t>Harry, Dylan</t>
+    <t>Dylan, Stephen</t>
   </si>
   <si>
     <t>T3</t>
@@ -112,7 +112,7 @@
     <t>Design and implement the graphical interface for both student and admin users.</t>
   </si>
   <si>
-    <t>Nathan, Harry</t>
+    <t>Nathan, Stephen, Harry</t>
   </si>
   <si>
     <t>T7</t>
@@ -136,7 +136,7 @@
     <t>Create reports that display course enrollment numbers, capacities, and overall statistics.</t>
   </si>
   <si>
-    <t>Harry, Zang</t>
+    <t>Zang</t>
   </si>
   <si>
     <t>T9</t>
@@ -148,7 +148,7 @@
     <t>Test each module for errors, fix bugs, and ensure system reliability before deployment.</t>
   </si>
   <si>
-    <t>Zang</t>
+    <t>Entire Team</t>
   </si>
   <si>
     <t>T10</t>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>The server will write and retrieve information from this file to maintain data persistence between sessions.</t>
-  </si>
-  <si>
-    <t>Harry</t>
   </si>
 </sst>
 </file>
@@ -472,7 +469,7 @@
         <v>45960.0</v>
       </c>
       <c r="F2" s="2">
-        <v>45994.0</v>
+        <v>45992.0</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>12</v>
@@ -498,7 +495,7 @@
         <v>45960.0</v>
       </c>
       <c r="F3" s="2">
-        <v>45994.0</v>
+        <v>45992.0</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
@@ -524,7 +521,7 @@
         <v>45960.0</v>
       </c>
       <c r="F4" s="2">
-        <v>45994.0</v>
+        <v>45992.0</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>12</v>
@@ -550,7 +547,7 @@
         <v>45960.0</v>
       </c>
       <c r="F5" s="2">
-        <v>45994.0</v>
+        <v>45992.0</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
@@ -576,7 +573,7 @@
         <v>45960.0</v>
       </c>
       <c r="F6" s="2">
-        <v>45994.0</v>
+        <v>45992.0</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
@@ -602,7 +599,7 @@
         <v>45960.0</v>
       </c>
       <c r="F7" s="2">
-        <v>45994.0</v>
+        <v>45992.0</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>12</v>
@@ -628,7 +625,7 @@
         <v>45960.0</v>
       </c>
       <c r="F8" s="2">
-        <v>45994.0</v>
+        <v>45992.0</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>12</v>
@@ -654,7 +651,7 @@
         <v>45960.0</v>
       </c>
       <c r="F9" s="2">
-        <v>45994.0</v>
+        <v>45992.0</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>12</v>
@@ -680,7 +677,7 @@
         <v>45960.0</v>
       </c>
       <c r="F10" s="2">
-        <v>45994.0</v>
+        <v>45992.0</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>12</v>
@@ -700,13 +697,13 @@
         <v>48</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2">
         <v>45960.0</v>
       </c>
       <c r="F11" s="2">
-        <v>45994.0</v>
+        <v>45992.0</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>12</v>

</xml_diff>